<commit_message>
Added control labels for the first page in the settings dialog.
</commit_message>
<xml_diff>
--- a/Files/Controls.xlsx
+++ b/Files/Controls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl-Otto\Documents\src\NVDA\vismaadministration-nvdaaddon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl-Otto\Documents\src\NVDA\VismaAdministration\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F26F91-2C72-47C2-B7B3-D32252871933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E157496-2BE6-48EB-BCF8-DA1D31F7C038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="16876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,30 +32,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="459">
   <si>
     <t>WindowClassName</t>
   </si>
@@ -552,9 +530,6 @@
     <t>Telefon 2</t>
   </si>
   <si>
-    <t>Fax</t>
-  </si>
-  <si>
     <t>Mobiltelefon</t>
   </si>
   <si>
@@ -678,9 +653,6 @@
     <t>Avvikande Leveransadress, telefon 3</t>
   </si>
   <si>
-    <t>Avvikande Leveransadress, fax</t>
-  </si>
-  <si>
     <t>Kundkategori</t>
   </si>
   <si>
@@ -1408,6 +1380,36 @@
   </si>
   <si>
     <t>Extra referenskod</t>
+  </si>
+  <si>
+    <t>Inställningar</t>
+  </si>
+  <si>
+    <t>Säte</t>
+  </si>
+  <si>
+    <t>Hemsida</t>
+  </si>
+  <si>
+    <t>Konto till bankgiro:</t>
+  </si>
+  <si>
+    <t>Branschkod (SNI)</t>
+  </si>
+  <si>
+    <t>VAT/Momsregistreringsnummer</t>
+  </si>
+  <si>
+    <t>Inhemskt språk</t>
+  </si>
+  <si>
+    <t>Inhemsk valuta</t>
+  </si>
+  <si>
+    <t>Koncernens orgnr:</t>
+  </si>
+  <si>
+    <t>Avvikande Leveransadress, Telefon 3</t>
   </si>
 </sst>
 </file>
@@ -1725,15 +1727,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E510"/>
+  <dimension ref="A1:E533"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D510" sqref="A1:E510"/>
+    <sheetView tabSelected="1" topLeftCell="A492" workbookViewId="0">
+      <selection activeCell="A534" sqref="A534"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="26.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
@@ -1741,7 +1744,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1761,7 +1764,7 @@
         <v>7407</v>
       </c>
       <c r="C2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
@@ -1775,10 +1778,10 @@
         <v>7407</v>
       </c>
       <c r="C3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -1789,10 +1792,10 @@
         <v>21346</v>
       </c>
       <c r="C4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -1803,10 +1806,10 @@
         <v>21346</v>
       </c>
       <c r="C5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -1817,10 +1820,10 @@
         <v>21346</v>
       </c>
       <c r="C6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -1831,10 +1834,10 @@
         <v>21346</v>
       </c>
       <c r="C7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -1845,10 +1848,10 @@
         <v>21346</v>
       </c>
       <c r="C8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -1859,10 +1862,10 @@
         <v>21211</v>
       </c>
       <c r="C9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -1873,10 +1876,10 @@
         <v>21346</v>
       </c>
       <c r="C10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -1887,10 +1890,10 @@
         <v>21346</v>
       </c>
       <c r="C11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -1901,10 +1904,10 @@
         <v>21516</v>
       </c>
       <c r="C12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
@@ -1915,10 +1918,10 @@
         <v>21516</v>
       </c>
       <c r="C13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
@@ -1929,10 +1932,10 @@
         <v>21516</v>
       </c>
       <c r="C14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
@@ -1943,10 +1946,10 @@
         <v>21516</v>
       </c>
       <c r="C15" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
@@ -1957,10 +1960,10 @@
         <v>21516</v>
       </c>
       <c r="C16" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
@@ -1971,10 +1974,10 @@
         <v>21516</v>
       </c>
       <c r="C17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
@@ -1985,10 +1988,10 @@
         <v>21516</v>
       </c>
       <c r="C18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
@@ -1999,10 +2002,10 @@
         <v>21577</v>
       </c>
       <c r="C19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
@@ -2013,10 +2016,10 @@
         <v>21629</v>
       </c>
       <c r="C20" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D20" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
@@ -2027,10 +2030,10 @@
         <v>24693</v>
       </c>
       <c r="C21" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
@@ -2041,10 +2044,10 @@
         <v>21666</v>
       </c>
       <c r="C22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
@@ -2055,25 +2058,24 @@
         <v>21769</v>
       </c>
       <c r="C23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D23" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" t="e" cm="1">
-        <f t="array" ref="A24">-SafGrid</f>
+      <c r="A24" t="e">
         <v>#NAME?</v>
       </c>
       <c r="B24">
         <v>21679</v>
       </c>
       <c r="C24" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E24" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
@@ -2084,10 +2086,10 @@
         <v>21666</v>
       </c>
       <c r="C25" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D25" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
@@ -2098,10 +2100,10 @@
         <v>21666</v>
       </c>
       <c r="C26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
@@ -2134,7 +2136,7 @@
         <v>7221</v>
       </c>
       <c r="D29" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
@@ -2145,7 +2147,7 @@
         <v>23569</v>
       </c>
       <c r="D30" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
@@ -2156,10 +2158,10 @@
         <v>21346</v>
       </c>
       <c r="C31" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D31" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
@@ -2170,7 +2172,7 @@
         <v>59648</v>
       </c>
       <c r="D32" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
@@ -2393,7 +2395,7 @@
         <v>20593</v>
       </c>
       <c r="D52" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
@@ -2578,7 +2580,7 @@
         <v>22308</v>
       </c>
       <c r="C68" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D68" t="s">
         <v>52</v>
@@ -2595,7 +2597,7 @@
         <v>22308</v>
       </c>
       <c r="C69" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D69" t="s">
         <v>53</v>
@@ -2609,7 +2611,7 @@
         <v>22308</v>
       </c>
       <c r="C70" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
@@ -2741,7 +2743,7 @@
         <v>22316</v>
       </c>
       <c r="C82" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D82" t="s">
         <v>65</v>
@@ -2755,7 +2757,7 @@
         <v>22316</v>
       </c>
       <c r="C83" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D83" t="s">
         <v>66</v>
@@ -2769,7 +2771,7 @@
         <v>22316</v>
       </c>
       <c r="C84" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D84" t="s">
         <v>67</v>
@@ -2783,7 +2785,7 @@
         <v>22317</v>
       </c>
       <c r="C85" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D85" t="s">
         <v>68</v>
@@ -2797,7 +2799,7 @@
         <v>22317</v>
       </c>
       <c r="C86" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D86" t="s">
         <v>69</v>
@@ -2811,7 +2813,7 @@
         <v>22317</v>
       </c>
       <c r="C87" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D87" t="s">
         <v>70</v>
@@ -2957,7 +2959,7 @@
         <v>22314</v>
       </c>
       <c r="C100" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D100" t="s">
         <v>82</v>
@@ -2971,7 +2973,7 @@
         <v>22314</v>
       </c>
       <c r="C101" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D101" t="s">
         <v>83</v>
@@ -3029,7 +3031,7 @@
         <v>24932</v>
       </c>
       <c r="C106" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D106" t="s">
         <v>88</v>
@@ -3043,7 +3045,7 @@
         <v>24932</v>
       </c>
       <c r="C107" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D107" t="s">
         <v>89</v>
@@ -3478,7 +3480,7 @@
         <v>22378</v>
       </c>
       <c r="C146" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D146" t="s">
         <v>129</v>
@@ -3495,7 +3497,7 @@
         <v>22378</v>
       </c>
       <c r="C147" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D147" t="s">
         <v>130</v>
@@ -3685,7 +3687,7 @@
         <v>22309</v>
       </c>
       <c r="C164" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D164" t="s">
         <v>148</v>
@@ -3702,7 +3704,7 @@
         <v>22309</v>
       </c>
       <c r="C165" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D165" t="s">
         <v>149</v>
@@ -3716,7 +3718,7 @@
         <v>22310</v>
       </c>
       <c r="C166" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D166" t="s">
         <v>150</v>
@@ -3730,7 +3732,7 @@
         <v>22310</v>
       </c>
       <c r="C167" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D167" t="s">
         <v>151</v>
@@ -3744,7 +3746,7 @@
         <v>22311</v>
       </c>
       <c r="C168" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D168" t="s">
         <v>152</v>
@@ -3758,7 +3760,7 @@
         <v>22311</v>
       </c>
       <c r="C169" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D169" t="s">
         <v>153</v>
@@ -3998,7 +4000,7 @@
         <v>23189</v>
       </c>
       <c r="D190" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.45">
@@ -4031,7 +4033,7 @@
         <v>20748</v>
       </c>
       <c r="D193" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.45">
@@ -4042,7 +4044,7 @@
         <v>24921</v>
       </c>
       <c r="D194" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.45">
@@ -4053,7 +4055,7 @@
         <v>23228</v>
       </c>
       <c r="D195" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.45">
@@ -4064,7 +4066,7 @@
         <v>23229</v>
       </c>
       <c r="D196" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.45">
@@ -4108,7 +4110,7 @@
         <v>26256</v>
       </c>
       <c r="D200" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.45">
@@ -4119,7 +4121,7 @@
         <v>23230</v>
       </c>
       <c r="D201" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.45">
@@ -4130,7 +4132,7 @@
         <v>23220</v>
       </c>
       <c r="D202" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.45">
@@ -4141,7 +4143,7 @@
         <v>23196</v>
       </c>
       <c r="D203" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.45">
@@ -4152,7 +4154,7 @@
         <v>23194</v>
       </c>
       <c r="D204" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.45">
@@ -4163,7 +4165,7 @@
         <v>23195</v>
       </c>
       <c r="D205" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.45">
@@ -4174,7 +4176,7 @@
         <v>21770</v>
       </c>
       <c r="D206" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.45">
@@ -4207,7 +4209,7 @@
         <v>23197</v>
       </c>
       <c r="D209" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.45">
@@ -4240,7 +4242,7 @@
         <v>26598</v>
       </c>
       <c r="D212" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.45">
@@ -4317,7 +4319,7 @@
         <v>24920</v>
       </c>
       <c r="D219" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.45">
@@ -4328,10 +4330,10 @@
         <v>23213</v>
       </c>
       <c r="D220" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E220" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.45">
@@ -4342,7 +4344,7 @@
         <v>23214</v>
       </c>
       <c r="D221" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.45">
@@ -4353,7 +4355,7 @@
         <v>23215</v>
       </c>
       <c r="D222" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.45">
@@ -4364,7 +4366,7 @@
         <v>23216</v>
       </c>
       <c r="D223" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.45">
@@ -4408,7 +4410,7 @@
         <v>23211</v>
       </c>
       <c r="D227" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.45">
@@ -4419,7 +4421,7 @@
         <v>23212</v>
       </c>
       <c r="D228" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.45">
@@ -4430,7 +4432,7 @@
         <v>23590</v>
       </c>
       <c r="D229" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.45">
@@ -4441,7 +4443,7 @@
         <v>23231</v>
       </c>
       <c r="D230" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.45">
@@ -4452,10 +4454,10 @@
         <v>24974</v>
       </c>
       <c r="D231" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E231" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.45">
@@ -4466,7 +4468,7 @@
         <v>24990</v>
       </c>
       <c r="D232" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.45">
@@ -4477,13 +4479,13 @@
         <v>22423</v>
       </c>
       <c r="C233" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D233" t="s">
         <v>54</v>
       </c>
       <c r="E233" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.45">
@@ -4494,13 +4496,13 @@
         <v>22423</v>
       </c>
       <c r="C234" t="s">
+        <v>275</v>
+      </c>
+      <c r="D234" t="s">
         <v>277</v>
       </c>
-      <c r="D234" t="s">
-        <v>279</v>
-      </c>
       <c r="E234" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.45">
@@ -4511,10 +4513,10 @@
         <v>22487</v>
       </c>
       <c r="C235" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D235" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.45">
@@ -4525,10 +4527,10 @@
         <v>22424</v>
       </c>
       <c r="C236" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D236" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.45">
@@ -4550,7 +4552,7 @@
         <v>22444</v>
       </c>
       <c r="C238" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D238" t="s">
         <v>160</v>
@@ -4564,10 +4566,10 @@
         <v>22444</v>
       </c>
       <c r="C239" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D239" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.45">
@@ -4578,7 +4580,7 @@
         <v>22426</v>
       </c>
       <c r="D240" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.45">
@@ -4699,7 +4701,7 @@
         <v>23628</v>
       </c>
       <c r="D251" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.45">
@@ -4710,7 +4712,7 @@
         <v>22433</v>
       </c>
       <c r="D252" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.45">
@@ -4743,7 +4745,7 @@
         <v>22443</v>
       </c>
       <c r="D255" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.45">
@@ -4754,7 +4756,7 @@
         <v>20747</v>
       </c>
       <c r="D256" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.45">
@@ -4765,7 +4767,7 @@
         <v>22485</v>
       </c>
       <c r="D257" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.45">
@@ -4776,7 +4778,7 @@
         <v>22434</v>
       </c>
       <c r="D258" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.45">
@@ -4787,7 +4789,7 @@
         <v>22435</v>
       </c>
       <c r="D259" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.45">
@@ -4798,7 +4800,7 @@
         <v>22544</v>
       </c>
       <c r="D260" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.45">
@@ -4809,7 +4811,7 @@
         <v>23735</v>
       </c>
       <c r="D261" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.45">
@@ -4820,7 +4822,7 @@
         <v>22436</v>
       </c>
       <c r="D262" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.45">
@@ -4831,7 +4833,7 @@
         <v>22437</v>
       </c>
       <c r="D263" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.45">
@@ -4842,7 +4844,7 @@
         <v>22438</v>
       </c>
       <c r="D264" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.45">
@@ -4853,7 +4855,7 @@
         <v>23601</v>
       </c>
       <c r="D265" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.45">
@@ -4864,7 +4866,7 @@
         <v>22439</v>
       </c>
       <c r="D266" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.45">
@@ -4875,7 +4877,7 @@
         <v>22440</v>
       </c>
       <c r="D267" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.45">
@@ -4886,7 +4888,7 @@
         <v>22441</v>
       </c>
       <c r="D268" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.45">
@@ -4897,7 +4899,7 @@
         <v>23626</v>
       </c>
       <c r="D269" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.45">
@@ -4908,7 +4910,7 @@
         <v>22442</v>
       </c>
       <c r="D270" t="s">
-        <v>207</v>
+        <v>458</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.45">
@@ -4919,10 +4921,10 @@
         <v>22446</v>
       </c>
       <c r="C271" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D271" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.45">
@@ -4933,10 +4935,10 @@
         <v>22446</v>
       </c>
       <c r="C272" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D272" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.45">
@@ -4947,10 +4949,10 @@
         <v>22587</v>
       </c>
       <c r="C273" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D273" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.45">
@@ -4961,10 +4963,10 @@
         <v>22588</v>
       </c>
       <c r="C274" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D274" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.45">
@@ -4975,10 +4977,10 @@
         <v>22589</v>
       </c>
       <c r="C275" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D275" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.45">
@@ -4989,10 +4991,10 @@
         <v>22590</v>
       </c>
       <c r="C276" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D276" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.45">
@@ -5003,10 +5005,10 @@
         <v>22591</v>
       </c>
       <c r="C277" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D277" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.45">
@@ -5017,10 +5019,10 @@
         <v>22592</v>
       </c>
       <c r="C278" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D278" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.45">
@@ -5031,10 +5033,10 @@
         <v>22593</v>
       </c>
       <c r="C279" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D279" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.45">
@@ -5045,10 +5047,10 @@
         <v>22594</v>
       </c>
       <c r="C280" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D280" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.45">
@@ -5059,10 +5061,10 @@
         <v>22595</v>
       </c>
       <c r="C281" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D281" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.45">
@@ -5073,10 +5075,10 @@
         <v>22596</v>
       </c>
       <c r="C282" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D282" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.45">
@@ -5087,10 +5089,10 @@
         <v>26572</v>
       </c>
       <c r="C283" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D283" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.45">
@@ -5126,7 +5128,7 @@
         <v>59</v>
       </c>
       <c r="E286" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.45">
@@ -5225,7 +5227,7 @@
         <v>22479</v>
       </c>
       <c r="D295" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.45">
@@ -5236,7 +5238,7 @@
         <v>22480</v>
       </c>
       <c r="D296" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.45">
@@ -5247,7 +5249,7 @@
         <v>22467</v>
       </c>
       <c r="D297" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.45">
@@ -5291,7 +5293,7 @@
         <v>22464</v>
       </c>
       <c r="D301" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.45">
@@ -5335,7 +5337,7 @@
         <v>26461</v>
       </c>
       <c r="D305" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.45">
@@ -5346,7 +5348,7 @@
         <v>26462</v>
       </c>
       <c r="D306" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.45">
@@ -5357,10 +5359,10 @@
         <v>24838</v>
       </c>
       <c r="D307" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E307" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.45">
@@ -5371,7 +5373,7 @@
         <v>24842</v>
       </c>
       <c r="D308" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.45">
@@ -5382,7 +5384,7 @@
         <v>24846</v>
       </c>
       <c r="D309" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.45">
@@ -5393,7 +5395,7 @@
         <v>24849</v>
       </c>
       <c r="D310" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.45">
@@ -5404,7 +5406,7 @@
         <v>24852</v>
       </c>
       <c r="D311" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.45">
@@ -5415,7 +5417,7 @@
         <v>24856</v>
       </c>
       <c r="D312" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.45">
@@ -5426,7 +5428,7 @@
         <v>24859</v>
       </c>
       <c r="D313" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.45">
@@ -5437,10 +5439,10 @@
         <v>7315</v>
       </c>
       <c r="D314" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E314" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.45">
@@ -5451,7 +5453,7 @@
         <v>7316</v>
       </c>
       <c r="D315" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.45">
@@ -5462,7 +5464,7 @@
         <v>6818</v>
       </c>
       <c r="D316" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.45">
@@ -5473,10 +5475,10 @@
         <v>23566</v>
       </c>
       <c r="D317" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E317" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.45">
@@ -5498,7 +5500,7 @@
         <v>24655</v>
       </c>
       <c r="D319" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.45">
@@ -5509,10 +5511,10 @@
         <v>23233</v>
       </c>
       <c r="D320" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E320" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.45">
@@ -5567,7 +5569,7 @@
         <v>23237</v>
       </c>
       <c r="D325" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.45">
@@ -5578,7 +5580,7 @@
         <v>23257</v>
       </c>
       <c r="D326" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.45">
@@ -5589,7 +5591,7 @@
         <v>23251</v>
       </c>
       <c r="D327" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.45">
@@ -5655,7 +5657,7 @@
         <v>23244</v>
       </c>
       <c r="D333" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.45">
@@ -5666,7 +5668,7 @@
         <v>25019</v>
       </c>
       <c r="D334" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.45">
@@ -5677,7 +5679,7 @@
         <v>24695</v>
       </c>
       <c r="C335" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D335" t="s">
         <v>55</v>
@@ -5691,10 +5693,10 @@
         <v>24694</v>
       </c>
       <c r="C336" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D336" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.45">
@@ -5705,10 +5707,10 @@
         <v>24696</v>
       </c>
       <c r="C337" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D337" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.45">
@@ -5719,7 +5721,7 @@
         <v>24697</v>
       </c>
       <c r="C338" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D338" t="s">
         <v>163</v>
@@ -5733,7 +5735,7 @@
         <v>24698</v>
       </c>
       <c r="C339" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D339" t="s">
         <v>164</v>
@@ -5747,10 +5749,10 @@
         <v>24699</v>
       </c>
       <c r="C340" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D340" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.45">
@@ -5761,10 +5763,10 @@
         <v>24700</v>
       </c>
       <c r="C341" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D341" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.45">
@@ -5775,7 +5777,7 @@
         <v>24701</v>
       </c>
       <c r="C342" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D342" t="s">
         <v>54</v>
@@ -5789,7 +5791,7 @@
         <v>24702</v>
       </c>
       <c r="C343" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D343" t="s">
         <v>159</v>
@@ -5803,10 +5805,10 @@
         <v>24703</v>
       </c>
       <c r="C344" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D344" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.45">
@@ -5817,7 +5819,7 @@
         <v>24704</v>
       </c>
       <c r="C345" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D345" t="s">
         <v>92</v>
@@ -5831,10 +5833,10 @@
         <v>24705</v>
       </c>
       <c r="C346" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D346" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.45">
@@ -5845,7 +5847,7 @@
         <v>24707</v>
       </c>
       <c r="C347" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D347" t="s">
         <v>162</v>
@@ -5859,7 +5861,7 @@
         <v>24708</v>
       </c>
       <c r="C348" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D348" t="s">
         <v>95</v>
@@ -5873,7 +5875,7 @@
         <v>24709</v>
       </c>
       <c r="C349" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D349" t="s">
         <v>96</v>
@@ -5887,7 +5889,7 @@
         <v>24711</v>
       </c>
       <c r="C350" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D350" t="s">
         <v>97</v>
@@ -5901,7 +5903,7 @@
         <v>24710</v>
       </c>
       <c r="C351" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D351" t="s">
         <v>98</v>
@@ -5915,10 +5917,10 @@
         <v>24706</v>
       </c>
       <c r="C352" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D352" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.45">
@@ -5929,10 +5931,10 @@
         <v>22175</v>
       </c>
       <c r="C353" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D353" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.45">
@@ -5943,7 +5945,7 @@
         <v>22176</v>
       </c>
       <c r="C354" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D354" t="s">
         <v>8</v>
@@ -5957,10 +5959,10 @@
         <v>22177</v>
       </c>
       <c r="C355" t="s">
+        <v>303</v>
+      </c>
+      <c r="D355" t="s">
         <v>305</v>
-      </c>
-      <c r="D355" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.45">
@@ -5971,10 +5973,10 @@
         <v>23591</v>
       </c>
       <c r="C356" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D356" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.45">
@@ -5985,10 +5987,10 @@
         <v>22178</v>
       </c>
       <c r="C357" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D357" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.45">
@@ -5999,10 +6001,10 @@
         <v>22180</v>
       </c>
       <c r="C358" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D358" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.45">
@@ -6013,10 +6015,10 @@
         <v>22179</v>
       </c>
       <c r="C359" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D359" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.45">
@@ -6027,10 +6029,10 @@
         <v>24903</v>
       </c>
       <c r="C360" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D360" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.45">
@@ -6041,7 +6043,7 @@
         <v>22183</v>
       </c>
       <c r="C361" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D361" t="s">
         <v>63</v>
@@ -6055,10 +6057,10 @@
         <v>22185</v>
       </c>
       <c r="C362" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D362" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.45">
@@ -6069,7 +6071,7 @@
         <v>22186</v>
       </c>
       <c r="C363" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D363" t="s">
         <v>64</v>
@@ -6083,10 +6085,10 @@
         <v>22188</v>
       </c>
       <c r="C364" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D364" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.45">
@@ -6097,10 +6099,10 @@
         <v>22189</v>
       </c>
       <c r="C365" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D365" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.45">
@@ -6111,10 +6113,10 @@
         <v>22191</v>
       </c>
       <c r="C366" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D366" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.45">
@@ -6125,10 +6127,10 @@
         <v>22192</v>
       </c>
       <c r="C367" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D367" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.45">
@@ -6139,10 +6141,10 @@
         <v>22194</v>
       </c>
       <c r="C368" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D368" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.45">
@@ -6153,10 +6155,10 @@
         <v>22195</v>
       </c>
       <c r="C369" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D369" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.45">
@@ -6167,10 +6169,10 @@
         <v>22196</v>
       </c>
       <c r="C370" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D370" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.45">
@@ -6181,10 +6183,10 @@
         <v>22198</v>
       </c>
       <c r="C371" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D371" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.45">
@@ -6195,10 +6197,10 @@
         <v>22301</v>
       </c>
       <c r="C372" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D372" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.45">
@@ -6209,10 +6211,10 @@
         <v>21164</v>
       </c>
       <c r="C373" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D373" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.45">
@@ -6223,10 +6225,10 @@
         <v>21167</v>
       </c>
       <c r="C374" t="s">
+        <v>320</v>
+      </c>
+      <c r="D374" t="s">
         <v>322</v>
-      </c>
-      <c r="D374" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.45">
@@ -6237,10 +6239,10 @@
         <v>22303</v>
       </c>
       <c r="C375" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D375" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.45">
@@ -6251,10 +6253,10 @@
         <v>22302</v>
       </c>
       <c r="C376" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D376" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.45">
@@ -6265,10 +6267,10 @@
         <v>26470</v>
       </c>
       <c r="C377" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D377" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.45">
@@ -6279,10 +6281,10 @@
         <v>24897</v>
       </c>
       <c r="C378" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D378" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.45">
@@ -6293,7 +6295,7 @@
         <v>24894</v>
       </c>
       <c r="C379" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D379" t="s">
         <v>63</v>
@@ -6307,7 +6309,7 @@
         <v>24895</v>
       </c>
       <c r="C380" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D380" t="s">
         <v>64</v>
@@ -6321,10 +6323,10 @@
         <v>25052</v>
       </c>
       <c r="C381" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D381" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.45">
@@ -6335,10 +6337,10 @@
         <v>23978</v>
       </c>
       <c r="C382" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D382" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.45">
@@ -6349,10 +6351,10 @@
         <v>23983</v>
       </c>
       <c r="C383" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D383" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.45">
@@ -6363,10 +6365,10 @@
         <v>23868</v>
       </c>
       <c r="C384" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D384" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.45">
@@ -6377,10 +6379,10 @@
         <v>23869</v>
       </c>
       <c r="C385" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D385" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.45">
@@ -6391,10 +6393,10 @@
         <v>23870</v>
       </c>
       <c r="C386" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D386" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.45">
@@ -6405,10 +6407,10 @@
         <v>23873</v>
       </c>
       <c r="C387" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D387" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.45">
@@ -6419,10 +6421,10 @@
         <v>23874</v>
       </c>
       <c r="C388" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D388" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.45">
@@ -6433,10 +6435,10 @@
         <v>23875</v>
       </c>
       <c r="C389" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D389" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.45">
@@ -6447,10 +6449,10 @@
         <v>23876</v>
       </c>
       <c r="C390" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D390" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.45">
@@ -6461,10 +6463,10 @@
         <v>23877</v>
       </c>
       <c r="C391" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D391" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.45">
@@ -6475,10 +6477,10 @@
         <v>23878</v>
       </c>
       <c r="C392" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D392" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.45">
@@ -6489,10 +6491,10 @@
         <v>23879</v>
       </c>
       <c r="C393" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D393" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.45">
@@ -6503,10 +6505,10 @@
         <v>23880</v>
       </c>
       <c r="C394" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D394" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.45">
@@ -6517,10 +6519,10 @@
         <v>23881</v>
       </c>
       <c r="C395" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D395" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.45">
@@ -6531,10 +6533,10 @@
         <v>23882</v>
       </c>
       <c r="C396" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D396" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.45">
@@ -6545,10 +6547,10 @@
         <v>23883</v>
       </c>
       <c r="C397" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D397" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.45">
@@ -6559,10 +6561,10 @@
         <v>23884</v>
       </c>
       <c r="C398" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D398" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.45">
@@ -6573,10 +6575,10 @@
         <v>23885</v>
       </c>
       <c r="C399" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D399" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.45">
@@ -6587,10 +6589,10 @@
         <v>23886</v>
       </c>
       <c r="C400" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D400" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.45">
@@ -6601,10 +6603,10 @@
         <v>26659</v>
       </c>
       <c r="C401" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D401" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.45">
@@ -6615,10 +6617,10 @@
         <v>23887</v>
       </c>
       <c r="C402" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D402" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.45">
@@ -6629,10 +6631,10 @@
         <v>24123</v>
       </c>
       <c r="C403" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D403" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.45">
@@ -6643,10 +6645,10 @@
         <v>26202</v>
       </c>
       <c r="C404" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D404" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.45">
@@ -6657,10 +6659,10 @@
         <v>26203</v>
       </c>
       <c r="C405" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D405" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.45">
@@ -6671,10 +6673,10 @@
         <v>23888</v>
       </c>
       <c r="C406" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D406" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.45">
@@ -6685,10 +6687,10 @@
         <v>23871</v>
       </c>
       <c r="C407" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D407" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.45">
@@ -6699,10 +6701,10 @@
         <v>23872</v>
       </c>
       <c r="C408" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D408" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.45">
@@ -6713,10 +6715,10 @@
         <v>24088</v>
       </c>
       <c r="C409" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D409" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.45">
@@ -6727,10 +6729,10 @@
         <v>23889</v>
       </c>
       <c r="C410" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D410" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.45">
@@ -6741,10 +6743,10 @@
         <v>23890</v>
       </c>
       <c r="C411" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D411" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.45">
@@ -6755,10 +6757,10 @@
         <v>23891</v>
       </c>
       <c r="C412" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D412" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.45">
@@ -6769,10 +6771,10 @@
         <v>24873</v>
       </c>
       <c r="C413" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D413" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.45">
@@ -6783,10 +6785,10 @@
         <v>24874</v>
       </c>
       <c r="C414" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D414" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.45">
@@ -6797,10 +6799,10 @@
         <v>24875</v>
       </c>
       <c r="C415" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D415" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.45">
@@ -6811,10 +6813,10 @@
         <v>24876</v>
       </c>
       <c r="C416" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D416" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.45">
@@ -6825,10 +6827,10 @@
         <v>24877</v>
       </c>
       <c r="C417" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D417" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.45">
@@ -6839,10 +6841,10 @@
         <v>24878</v>
       </c>
       <c r="C418" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D418" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.45">
@@ -6853,10 +6855,10 @@
         <v>24879</v>
       </c>
       <c r="C419" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D419" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.45">
@@ -6867,10 +6869,10 @@
         <v>24089</v>
       </c>
       <c r="C420" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D420" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.45">
@@ -6881,10 +6883,10 @@
         <v>23892</v>
       </c>
       <c r="C421" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D421" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.45">
@@ -6895,10 +6897,10 @@
         <v>24095</v>
       </c>
       <c r="C422" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D422" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.45">
@@ -6909,10 +6911,10 @@
         <v>24174</v>
       </c>
       <c r="C423" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D423" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.45">
@@ -6923,10 +6925,10 @@
         <v>23893</v>
       </c>
       <c r="C424" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D424" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.45">
@@ -6937,10 +6939,10 @@
         <v>23894</v>
       </c>
       <c r="C425" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D425" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.45">
@@ -6951,10 +6953,10 @@
         <v>23895</v>
       </c>
       <c r="C426" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D426" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.45">
@@ -6965,10 +6967,10 @@
         <v>23984</v>
       </c>
       <c r="C427" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D427" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.45">
@@ -6979,10 +6981,10 @@
         <v>23985</v>
       </c>
       <c r="C428" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D428" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.45">
@@ -6993,10 +6995,10 @@
         <v>24090</v>
       </c>
       <c r="C429" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D429" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.45">
@@ -7007,10 +7009,10 @@
         <v>25007</v>
       </c>
       <c r="C430" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D430" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.45">
@@ -7021,10 +7023,10 @@
         <v>23988</v>
       </c>
       <c r="C431" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D431" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.45">
@@ -7035,10 +7037,10 @@
         <v>24038</v>
       </c>
       <c r="C432" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D432" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.45">
@@ -7049,10 +7051,10 @@
         <v>23987</v>
       </c>
       <c r="C433" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D433" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.45">
@@ -7063,10 +7065,10 @@
         <v>25003</v>
       </c>
       <c r="C434" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D434" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.45">
@@ -7077,10 +7079,10 @@
         <v>24085</v>
       </c>
       <c r="C435" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D435" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.45">
@@ -7091,10 +7093,10 @@
         <v>25004</v>
       </c>
       <c r="C436" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D436" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.45">
@@ -7105,10 +7107,10 @@
         <v>23989</v>
       </c>
       <c r="C437" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D437" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.45">
@@ -7119,10 +7121,10 @@
         <v>24032</v>
       </c>
       <c r="C438" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D438" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.45">
@@ -7133,10 +7135,10 @@
         <v>23990</v>
       </c>
       <c r="C439" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D439" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.45">
@@ -7147,10 +7149,10 @@
         <v>24034</v>
       </c>
       <c r="C440" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D440" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.45">
@@ -7161,10 +7163,10 @@
         <v>23991</v>
       </c>
       <c r="C441" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D441" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.45">
@@ -7175,10 +7177,10 @@
         <v>24036</v>
       </c>
       <c r="C442" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D442" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.45">
@@ -7189,10 +7191,10 @@
         <v>24086</v>
       </c>
       <c r="C443" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D443" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.45">
@@ -7203,10 +7205,10 @@
         <v>25005</v>
       </c>
       <c r="C444" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D444" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.45">
@@ -7217,10 +7219,10 @@
         <v>24087</v>
       </c>
       <c r="C445" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D445" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.45">
@@ -7231,10 +7233,10 @@
         <v>25006</v>
       </c>
       <c r="C446" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D446" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.45">
@@ -7245,10 +7247,10 @@
         <v>23986</v>
       </c>
       <c r="C447" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D447" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.45">
@@ -7259,10 +7261,10 @@
         <v>24092</v>
       </c>
       <c r="C448" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D448" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.45">
@@ -7273,10 +7275,10 @@
         <v>24093</v>
       </c>
       <c r="C449" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D449" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.45">
@@ -7287,10 +7289,10 @@
         <v>24094</v>
       </c>
       <c r="C450" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D450" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.45">
@@ -7301,10 +7303,10 @@
         <v>23896</v>
       </c>
       <c r="C451" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D451" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.45">
@@ -7315,10 +7317,10 @@
         <v>22248</v>
       </c>
       <c r="C452" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D452" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.45">
@@ -7329,10 +7331,10 @@
         <v>22251</v>
       </c>
       <c r="C453" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D453" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.45">
@@ -7343,10 +7345,10 @@
         <v>20743</v>
       </c>
       <c r="C454" t="s">
+        <v>398</v>
+      </c>
+      <c r="D454" t="s">
         <v>400</v>
-      </c>
-      <c r="D454" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.45">
@@ -7357,10 +7359,10 @@
         <v>20723</v>
       </c>
       <c r="C455" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D455" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.45">
@@ -7371,10 +7373,10 @@
         <v>20723</v>
       </c>
       <c r="C456" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D456" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.45">
@@ -7385,10 +7387,10 @@
         <v>21147</v>
       </c>
       <c r="C457" t="s">
+        <v>402</v>
+      </c>
+      <c r="D457" t="s">
         <v>404</v>
-      </c>
-      <c r="D457" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.45">
@@ -7399,10 +7401,10 @@
         <v>21146</v>
       </c>
       <c r="C458" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D458" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.45">
@@ -7413,10 +7415,10 @@
         <v>21148</v>
       </c>
       <c r="C459" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D459" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.45">
@@ -7427,10 +7429,10 @@
         <v>21149</v>
       </c>
       <c r="C460" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D460" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.45">
@@ -7441,10 +7443,10 @@
         <v>21150</v>
       </c>
       <c r="C461" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D461" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.45">
@@ -7455,10 +7457,10 @@
         <v>21151</v>
       </c>
       <c r="C462" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D462" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.45">
@@ -7469,10 +7471,10 @@
         <v>23637</v>
       </c>
       <c r="C463" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D463" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.45">
@@ -7483,10 +7485,10 @@
         <v>23638</v>
       </c>
       <c r="C464" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D464" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.45">
@@ -7497,10 +7499,10 @@
         <v>20723</v>
       </c>
       <c r="C465" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D465" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.45">
@@ -7511,10 +7513,10 @@
         <v>22084</v>
       </c>
       <c r="C466" t="s">
+        <v>413</v>
+      </c>
+      <c r="D466" t="s">
         <v>415</v>
-      </c>
-      <c r="D466" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.45">
@@ -7525,10 +7527,10 @@
         <v>22085</v>
       </c>
       <c r="C467" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D467" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.45">
@@ -7539,10 +7541,10 @@
         <v>24908</v>
       </c>
       <c r="C468" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D468" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.45">
@@ -7553,10 +7555,10 @@
         <v>21346</v>
       </c>
       <c r="C469" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D469" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.45">
@@ -7567,10 +7569,10 @@
         <v>26662</v>
       </c>
       <c r="C470" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D470" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.45">
@@ -7581,10 +7583,10 @@
         <v>21530</v>
       </c>
       <c r="C471" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D471" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.45">
@@ -7595,10 +7597,10 @@
         <v>21521</v>
       </c>
       <c r="C472" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D472" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.45">
@@ -7609,10 +7611,10 @@
         <v>22206</v>
       </c>
       <c r="C473" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D473" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.45">
@@ -7623,7 +7625,7 @@
         <v>22207</v>
       </c>
       <c r="C474" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D474" t="s">
         <v>55</v>
@@ -7637,10 +7639,10 @@
         <v>22208</v>
       </c>
       <c r="C475" t="s">
+        <v>422</v>
+      </c>
+      <c r="D475" t="s">
         <v>424</v>
-      </c>
-      <c r="D475" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.45">
@@ -7651,10 +7653,10 @@
         <v>22209</v>
       </c>
       <c r="C476" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D476" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.45">
@@ -7665,7 +7667,7 @@
         <v>22212</v>
       </c>
       <c r="C477" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D477" t="s">
         <v>54</v>
@@ -7679,10 +7681,10 @@
         <v>22213</v>
       </c>
       <c r="C478" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D478" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.45">
@@ -7693,10 +7695,10 @@
         <v>22215</v>
       </c>
       <c r="C479" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D479" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.45">
@@ -7707,10 +7709,10 @@
         <v>22216</v>
       </c>
       <c r="C480" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D480" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.45">
@@ -7721,7 +7723,7 @@
         <v>22217</v>
       </c>
       <c r="C481" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D481" t="s">
         <v>163</v>
@@ -7735,10 +7737,10 @@
         <v>22218</v>
       </c>
       <c r="C482" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D482" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.45">
@@ -7749,10 +7751,10 @@
         <v>22219</v>
       </c>
       <c r="C483" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D483" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.45">
@@ -7763,10 +7765,10 @@
         <v>22220</v>
       </c>
       <c r="C484" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D484" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.45">
@@ -7777,10 +7779,10 @@
         <v>22214</v>
       </c>
       <c r="C485" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D485" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.45">
@@ -7791,10 +7793,10 @@
         <v>22225</v>
       </c>
       <c r="C486" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D486" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.45">
@@ -7805,10 +7807,10 @@
         <v>22211</v>
       </c>
       <c r="C487" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D487" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.45">
@@ -7819,10 +7821,10 @@
         <v>22221</v>
       </c>
       <c r="C488" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D488" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.45">
@@ -7833,10 +7835,10 @@
         <v>22222</v>
       </c>
       <c r="C489" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D489" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.45">
@@ -7847,10 +7849,10 @@
         <v>22223</v>
       </c>
       <c r="C490" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D490" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.45">
@@ -7861,10 +7863,10 @@
         <v>22224</v>
       </c>
       <c r="C491" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D491" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.45">
@@ -7875,7 +7877,7 @@
         <v>22756</v>
       </c>
       <c r="C492" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D492" t="s">
         <v>159</v>
@@ -7889,7 +7891,7 @@
         <v>22757</v>
       </c>
       <c r="C493" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D493" t="s">
         <v>55</v>
@@ -7903,10 +7905,10 @@
         <v>22759</v>
       </c>
       <c r="C494" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D494" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.45">
@@ -7917,10 +7919,10 @@
         <v>22761</v>
       </c>
       <c r="C495" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D495" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.45">
@@ -7931,10 +7933,10 @@
         <v>22760</v>
       </c>
       <c r="C496" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D496" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.45">
@@ -7945,7 +7947,7 @@
         <v>22767</v>
       </c>
       <c r="C497" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D497" t="s">
         <v>63</v>
@@ -7959,7 +7961,7 @@
         <v>22766</v>
       </c>
       <c r="C498" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D498" t="s">
         <v>64</v>
@@ -7973,10 +7975,10 @@
         <v>22763</v>
       </c>
       <c r="C499" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D499" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="500" spans="1:4" x14ac:dyDescent="0.45">
@@ -7987,10 +7989,10 @@
         <v>22764</v>
       </c>
       <c r="C500" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D500" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.45">
@@ -8001,10 +8003,10 @@
         <v>22765</v>
       </c>
       <c r="C501" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D501" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="502" spans="1:4" x14ac:dyDescent="0.45">
@@ -8015,10 +8017,10 @@
         <v>21557</v>
       </c>
       <c r="C502" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D502" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.45">
@@ -8029,10 +8031,10 @@
         <v>21521</v>
       </c>
       <c r="C503" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D503" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.45">
@@ -8043,7 +8045,7 @@
         <v>21547</v>
       </c>
       <c r="C504" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.45">
@@ -8054,10 +8056,10 @@
         <v>23660</v>
       </c>
       <c r="C505" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D505" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.45">
@@ -8068,10 +8070,10 @@
         <v>23661</v>
       </c>
       <c r="C506" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D506" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.45">
@@ -8082,7 +8084,7 @@
         <v>23649</v>
       </c>
       <c r="C507" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D507" t="s">
         <v>95</v>
@@ -8096,7 +8098,7 @@
         <v>23650</v>
       </c>
       <c r="C508" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D508" t="s">
         <v>96</v>
@@ -8110,10 +8112,10 @@
         <v>26707</v>
       </c>
       <c r="C509" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D509" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="510" spans="1:4" x14ac:dyDescent="0.45">
@@ -8124,10 +8126,332 @@
         <v>26707</v>
       </c>
       <c r="C510" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D510" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A511" t="s">
+        <v>6</v>
+      </c>
+      <c r="B511">
+        <v>21863</v>
+      </c>
+      <c r="C511" t="s">
+        <v>449</v>
+      </c>
+      <c r="D511" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A512" t="s">
+        <v>6</v>
+      </c>
+      <c r="B512">
+        <v>21864</v>
+      </c>
+      <c r="C512" t="s">
+        <v>449</v>
+      </c>
+      <c r="D512" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="513" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A513" t="s">
+        <v>6</v>
+      </c>
+      <c r="B513">
+        <v>23728</v>
+      </c>
+      <c r="C513" t="s">
+        <v>449</v>
+      </c>
+      <c r="D513" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="514" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A514" t="s">
+        <v>6</v>
+      </c>
+      <c r="B514">
+        <v>21865</v>
+      </c>
+      <c r="C514" t="s">
+        <v>449</v>
+      </c>
+      <c r="D514" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="515" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A515" t="s">
+        <v>6</v>
+      </c>
+      <c r="B515">
+        <v>21866</v>
+      </c>
+      <c r="C515" t="s">
+        <v>449</v>
+      </c>
+      <c r="D515" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="516" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A516" t="s">
+        <v>6</v>
+      </c>
+      <c r="B516">
+        <v>21867</v>
+      </c>
+      <c r="C516" t="s">
+        <v>449</v>
+      </c>
+      <c r="D516" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="517" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A517" t="s">
+        <v>6</v>
+      </c>
+      <c r="B517">
+        <v>23974</v>
+      </c>
+      <c r="C517" t="s">
+        <v>449</v>
+      </c>
+      <c r="D517" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="518" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A518" t="s">
+        <v>6</v>
+      </c>
+      <c r="B518">
+        <v>21868</v>
+      </c>
+      <c r="C518" t="s">
+        <v>449</v>
+      </c>
+      <c r="D518" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="519" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A519" t="s">
+        <v>6</v>
+      </c>
+      <c r="B519">
+        <v>22053</v>
+      </c>
+      <c r="C519" t="s">
+        <v>449</v>
+      </c>
+      <c r="D519" t="s">
         <v>450</v>
+      </c>
+    </row>
+    <row r="520" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A520" t="s">
+        <v>6</v>
+      </c>
+      <c r="B520">
+        <v>21869</v>
+      </c>
+      <c r="C520" t="s">
+        <v>449</v>
+      </c>
+      <c r="D520" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="521" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A521" t="s">
+        <v>6</v>
+      </c>
+      <c r="B521">
+        <v>21870</v>
+      </c>
+      <c r="C521" t="s">
+        <v>449</v>
+      </c>
+      <c r="D521" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="522" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A522" t="s">
+        <v>6</v>
+      </c>
+      <c r="B522">
+        <v>21871</v>
+      </c>
+      <c r="C522" t="s">
+        <v>449</v>
+      </c>
+      <c r="D522" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="523" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A523" t="s">
+        <v>6</v>
+      </c>
+      <c r="B523">
+        <v>22048</v>
+      </c>
+      <c r="C523" t="s">
+        <v>449</v>
+      </c>
+      <c r="D523" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="524" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A524" t="s">
+        <v>6</v>
+      </c>
+      <c r="B524">
+        <v>22049</v>
+      </c>
+      <c r="C524" t="s">
+        <v>449</v>
+      </c>
+      <c r="D524" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="525" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A525" t="s">
+        <v>6</v>
+      </c>
+      <c r="B525">
+        <v>21874</v>
+      </c>
+      <c r="C525" t="s">
+        <v>449</v>
+      </c>
+      <c r="D525" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="526" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A526" t="s">
+        <v>6</v>
+      </c>
+      <c r="B526">
+        <v>21981</v>
+      </c>
+      <c r="C526" t="s">
+        <v>449</v>
+      </c>
+      <c r="D526" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="527" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A527" t="s">
+        <v>6</v>
+      </c>
+      <c r="B527">
+        <v>21984</v>
+      </c>
+      <c r="C527" t="s">
+        <v>449</v>
+      </c>
+      <c r="D527" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="528" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A528" t="s">
+        <v>6</v>
+      </c>
+      <c r="B528">
+        <v>21873</v>
+      </c>
+      <c r="C528" t="s">
+        <v>449</v>
+      </c>
+      <c r="D528" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="529" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A529" t="s">
+        <v>6</v>
+      </c>
+      <c r="B529">
+        <v>21872</v>
+      </c>
+      <c r="C529" t="s">
+        <v>449</v>
+      </c>
+      <c r="D529" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="530" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A530" t="s">
+        <v>6</v>
+      </c>
+      <c r="B530">
+        <v>24649</v>
+      </c>
+      <c r="C530" t="s">
+        <v>449</v>
+      </c>
+      <c r="D530" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="531" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A531" t="s">
+        <v>6</v>
+      </c>
+      <c r="B531">
+        <v>21941</v>
+      </c>
+      <c r="C531" t="s">
+        <v>449</v>
+      </c>
+      <c r="D531" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="532" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A532" t="s">
+        <v>6</v>
+      </c>
+      <c r="B532">
+        <v>21942</v>
+      </c>
+      <c r="C532" t="s">
+        <v>449</v>
+      </c>
+      <c r="D532" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="533" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A533" t="s">
+        <v>6</v>
+      </c>
+      <c r="B533">
+        <v>26701</v>
+      </c>
+      <c r="C533" t="s">
+        <v>449</v>
+      </c>
+      <c r="D533" t="s">
+        <v>457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added labels for agreements.
</commit_message>
<xml_diff>
--- a/Files/Controls.xlsx
+++ b/Files/Controls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl-Otto\Documents\src\NVDA\VismaAdministration\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E157496-2BE6-48EB-BCF8-DA1D31F7C038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFCAFCB-5A98-4993-9F11-9A1CF3EE24B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="16876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="465">
   <si>
     <t>WindowClassName</t>
   </si>
@@ -1410,6 +1410,24 @@
   </si>
   <si>
     <t>Avvikande Leveransadress, Telefon 3</t>
+  </si>
+  <si>
+    <t>Avtalstid från och med</t>
+  </si>
+  <si>
+    <t>Avtalstid till och med</t>
+  </si>
+  <si>
+    <t>Första faktureringsmånad</t>
+  </si>
+  <si>
+    <t>Fakturadag</t>
+  </si>
+  <si>
+    <t>Fakturaintervall, månader</t>
+  </si>
+  <si>
+    <t>Nästa period, slut</t>
   </si>
 </sst>
 </file>
@@ -1727,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E533"/>
+  <dimension ref="A1:E543"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A492" workbookViewId="0">
-      <selection activeCell="A534" sqref="A534"/>
+    <sheetView tabSelected="1" topLeftCell="A501" workbookViewId="0">
+      <selection activeCell="A543" sqref="A543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8454,6 +8472,146 @@
         <v>457</v>
       </c>
     </row>
+    <row r="534" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A534" t="s">
+        <v>6</v>
+      </c>
+      <c r="B534">
+        <v>22554</v>
+      </c>
+      <c r="C534" t="s">
+        <v>234</v>
+      </c>
+      <c r="D534" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="535" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A535" t="s">
+        <v>6</v>
+      </c>
+      <c r="B535">
+        <v>22555</v>
+      </c>
+      <c r="C535" t="s">
+        <v>234</v>
+      </c>
+      <c r="D535" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="536" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A536" t="s">
+        <v>6</v>
+      </c>
+      <c r="B536">
+        <v>22316</v>
+      </c>
+      <c r="C536" t="s">
+        <v>234</v>
+      </c>
+      <c r="D536" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="537" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A537" t="s">
+        <v>6</v>
+      </c>
+      <c r="B537">
+        <v>22556</v>
+      </c>
+      <c r="C537" t="s">
+        <v>234</v>
+      </c>
+      <c r="D537" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="538" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A538" t="s">
+        <v>6</v>
+      </c>
+      <c r="B538">
+        <v>22554</v>
+      </c>
+      <c r="C538" t="s">
+        <v>234</v>
+      </c>
+      <c r="D538" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="539" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A539" t="s">
+        <v>6</v>
+      </c>
+      <c r="B539">
+        <v>22555</v>
+      </c>
+      <c r="C539" t="s">
+        <v>234</v>
+      </c>
+      <c r="D539" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="540" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A540" t="s">
+        <v>6</v>
+      </c>
+      <c r="B540">
+        <v>22556</v>
+      </c>
+      <c r="C540" t="s">
+        <v>234</v>
+      </c>
+      <c r="D540" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="541" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A541" t="s">
+        <v>6</v>
+      </c>
+      <c r="B541">
+        <v>22558</v>
+      </c>
+      <c r="C541" t="s">
+        <v>234</v>
+      </c>
+      <c r="D541" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="542" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A542" t="s">
+        <v>6</v>
+      </c>
+      <c r="B542">
+        <v>22557</v>
+      </c>
+      <c r="C542" t="s">
+        <v>234</v>
+      </c>
+      <c r="D542" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="543" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A543" t="s">
+        <v>6</v>
+      </c>
+      <c r="B543">
+        <v>22564</v>
+      </c>
+      <c r="C543" t="s">
+        <v>234</v>
+      </c>
+      <c r="D543" t="s">
+        <v>464</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated files for the latest add-on template.
</commit_message>
<xml_diff>
--- a/Files/Controls.xlsx
+++ b/Files/Controls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl-Otto\Documents\src\NVDA\VismaAdministration\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\NVDA\VismaAdministration\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2861600-8B09-409D-9027-E4BAB7602282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CCD753-4A51-4432-93DD-97CF5978B0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3308" yWindow="3308" windowWidth="23040" windowHeight="12232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4995" yWindow="4448" windowWidth="23040" windowHeight="12232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="471">
   <si>
     <t>WindowClassName</t>
   </si>
@@ -1763,10 +1763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E547"/>
+  <dimension ref="A1:E548"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A516" workbookViewId="0">
-      <selection activeCell="A547" sqref="A547:XFD547"/>
+    <sheetView tabSelected="1" topLeftCell="A518" workbookViewId="0">
+      <selection activeCell="D548" sqref="D548"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8686,6 +8686,20 @@
         <v>470</v>
       </c>
     </row>
+    <row r="548" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A548" t="s">
+        <v>6</v>
+      </c>
+      <c r="B548">
+        <v>24748</v>
+      </c>
+      <c r="C548" t="s">
+        <v>252</v>
+      </c>
+      <c r="D548" t="s">
+        <v>296</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added labels for bookings.
</commit_message>
<xml_diff>
--- a/Files/Controls.xlsx
+++ b/Files/Controls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\NVDA\VismaAdministration\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CCD753-4A51-4432-93DD-97CF5978B0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C7CBC2-89B6-4BAE-B305-F7AE47CCEA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4995" yWindow="4448" windowWidth="23040" windowHeight="12232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="16876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="486">
   <si>
     <t>WindowClassName</t>
   </si>
@@ -1446,6 +1446,51 @@
   </si>
   <si>
     <t>Strukturartiklar</t>
+  </si>
+  <si>
+    <t>Leverantörens namn</t>
+  </si>
+  <si>
+    <t>Projekt:</t>
+  </si>
+  <si>
+    <t>Beställningsdatum</t>
+  </si>
+  <si>
+    <t>Leverantörens ordernummer</t>
+  </si>
+  <si>
+    <t>Skickad</t>
+  </si>
+  <si>
+    <t>Avvik. Namn</t>
+  </si>
+  <si>
+    <t>Avvik. Postadress</t>
+  </si>
+  <si>
+    <t>Avvik. Postadress 2</t>
+  </si>
+  <si>
+    <t>Avvik. GLN</t>
+  </si>
+  <si>
+    <t>Avvik. Postnummer</t>
+  </si>
+  <si>
+    <t>Avvik. Ort</t>
+  </si>
+  <si>
+    <t>Avvik. Besöksadress</t>
+  </si>
+  <si>
+    <t>Avvik. Landskod</t>
+  </si>
+  <si>
+    <t>Artiklar</t>
+  </si>
+  <si>
+    <t>Spårningsval</t>
   </si>
 </sst>
 </file>
@@ -1763,10 +1808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E548"/>
+  <dimension ref="A1:E585"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A518" workbookViewId="0">
-      <selection activeCell="D548" sqref="D548"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D585" sqref="A1:E585"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8700,6 +8745,524 @@
         <v>296</v>
       </c>
     </row>
+    <row r="549" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A549" t="s">
+        <v>6</v>
+      </c>
+      <c r="B549">
+        <v>22770</v>
+      </c>
+      <c r="C549" t="s">
+        <v>247</v>
+      </c>
+      <c r="D549" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="550" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A550" t="s">
+        <v>6</v>
+      </c>
+      <c r="B550">
+        <v>22772</v>
+      </c>
+      <c r="C550" t="s">
+        <v>247</v>
+      </c>
+      <c r="D550" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="551" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A551" t="s">
+        <v>6</v>
+      </c>
+      <c r="B551">
+        <v>22793</v>
+      </c>
+      <c r="C551" t="s">
+        <v>247</v>
+      </c>
+      <c r="D551" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="552" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A552" t="s">
+        <v>6</v>
+      </c>
+      <c r="B552">
+        <v>22807</v>
+      </c>
+      <c r="C552" t="s">
+        <v>247</v>
+      </c>
+      <c r="D552" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="553" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A553" t="s">
+        <v>6</v>
+      </c>
+      <c r="B553">
+        <v>22794</v>
+      </c>
+      <c r="C553" t="s">
+        <v>247</v>
+      </c>
+      <c r="D553" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="554" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A554" t="s">
+        <v>6</v>
+      </c>
+      <c r="B554">
+        <v>22798</v>
+      </c>
+      <c r="C554" t="s">
+        <v>247</v>
+      </c>
+      <c r="D554" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="555" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A555" t="s">
+        <v>6</v>
+      </c>
+      <c r="B555">
+        <v>22797</v>
+      </c>
+      <c r="C555" t="s">
+        <v>247</v>
+      </c>
+      <c r="D555" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="556" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A556" t="s">
+        <v>6</v>
+      </c>
+      <c r="B556">
+        <v>22795</v>
+      </c>
+      <c r="C556" t="s">
+        <v>247</v>
+      </c>
+      <c r="D556" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="557" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A557" t="s">
+        <v>6</v>
+      </c>
+      <c r="B557">
+        <v>22796</v>
+      </c>
+      <c r="C557" t="s">
+        <v>247</v>
+      </c>
+      <c r="D557" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="558" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A558" t="s">
+        <v>6</v>
+      </c>
+      <c r="B558">
+        <v>22788</v>
+      </c>
+      <c r="C558" t="s">
+        <v>247</v>
+      </c>
+      <c r="D558" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="559" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A559" t="s">
+        <v>19</v>
+      </c>
+      <c r="B559">
+        <v>22792</v>
+      </c>
+      <c r="C559" t="s">
+        <v>247</v>
+      </c>
+      <c r="D559" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="560" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A560" t="s">
+        <v>6</v>
+      </c>
+      <c r="B560">
+        <v>22770</v>
+      </c>
+      <c r="C560" t="s">
+        <v>247</v>
+      </c>
+      <c r="D560" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="561" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A561" t="s">
+        <v>6</v>
+      </c>
+      <c r="B561">
+        <v>22772</v>
+      </c>
+      <c r="C561" t="s">
+        <v>247</v>
+      </c>
+      <c r="D561" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="562" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A562" t="s">
+        <v>6</v>
+      </c>
+      <c r="B562">
+        <v>22774</v>
+      </c>
+      <c r="C562" t="s">
+        <v>247</v>
+      </c>
+      <c r="D562" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="563" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A563" t="s">
+        <v>6</v>
+      </c>
+      <c r="B563">
+        <v>23170</v>
+      </c>
+      <c r="C563" t="s">
+        <v>247</v>
+      </c>
+      <c r="D563" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="564" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A564" t="s">
+        <v>6</v>
+      </c>
+      <c r="B564">
+        <v>23730</v>
+      </c>
+      <c r="C564" t="s">
+        <v>247</v>
+      </c>
+      <c r="D564" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="565" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A565" t="s">
+        <v>6</v>
+      </c>
+      <c r="B565">
+        <v>22776</v>
+      </c>
+      <c r="C565" t="s">
+        <v>247</v>
+      </c>
+      <c r="D565" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="566" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A566" t="s">
+        <v>6</v>
+      </c>
+      <c r="B566">
+        <v>22777</v>
+      </c>
+      <c r="C566" t="s">
+        <v>247</v>
+      </c>
+      <c r="D566" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="567" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A567" t="s">
+        <v>6</v>
+      </c>
+      <c r="B567">
+        <v>23598</v>
+      </c>
+      <c r="C567" t="s">
+        <v>247</v>
+      </c>
+      <c r="D567" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="568" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A568" t="s">
+        <v>6</v>
+      </c>
+      <c r="B568">
+        <v>22778</v>
+      </c>
+      <c r="C568" t="s">
+        <v>247</v>
+      </c>
+      <c r="D568" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="569" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A569" t="s">
+        <v>6</v>
+      </c>
+      <c r="B569">
+        <v>22804</v>
+      </c>
+      <c r="C569" t="s">
+        <v>247</v>
+      </c>
+      <c r="D569" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="570" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A570" t="s">
+        <v>6</v>
+      </c>
+      <c r="B570">
+        <v>22786</v>
+      </c>
+      <c r="C570" t="s">
+        <v>247</v>
+      </c>
+      <c r="D570" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="571" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A571" t="s">
+        <v>6</v>
+      </c>
+      <c r="B571">
+        <v>22787</v>
+      </c>
+      <c r="C571" t="s">
+        <v>247</v>
+      </c>
+      <c r="D571" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="572" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A572" t="s">
+        <v>6</v>
+      </c>
+      <c r="B572">
+        <v>22779</v>
+      </c>
+      <c r="C572" t="s">
+        <v>247</v>
+      </c>
+      <c r="D572" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="573" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A573" t="s">
+        <v>6</v>
+      </c>
+      <c r="B573">
+        <v>22780</v>
+      </c>
+      <c r="C573" t="s">
+        <v>247</v>
+      </c>
+      <c r="D573" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="574" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A574" t="s">
+        <v>6</v>
+      </c>
+      <c r="B574">
+        <v>23172</v>
+      </c>
+      <c r="C574" t="s">
+        <v>247</v>
+      </c>
+      <c r="D574" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="575" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A575" t="s">
+        <v>6</v>
+      </c>
+      <c r="B575">
+        <v>23731</v>
+      </c>
+      <c r="C575" t="s">
+        <v>247</v>
+      </c>
+      <c r="D575" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="576" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A576" t="s">
+        <v>6</v>
+      </c>
+      <c r="B576">
+        <v>22781</v>
+      </c>
+      <c r="C576" t="s">
+        <v>247</v>
+      </c>
+      <c r="D576" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="577" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A577" t="s">
+        <v>6</v>
+      </c>
+      <c r="B577">
+        <v>22783</v>
+      </c>
+      <c r="C577" t="s">
+        <v>247</v>
+      </c>
+      <c r="D577" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="578" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A578" t="s">
+        <v>6</v>
+      </c>
+      <c r="B578">
+        <v>22782</v>
+      </c>
+      <c r="C578" t="s">
+        <v>247</v>
+      </c>
+      <c r="D578" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="579" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A579" t="s">
+        <v>6</v>
+      </c>
+      <c r="B579">
+        <v>23599</v>
+      </c>
+      <c r="C579" t="s">
+        <v>247</v>
+      </c>
+      <c r="D579" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="580" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A580" t="s">
+        <v>6</v>
+      </c>
+      <c r="B580">
+        <v>22784</v>
+      </c>
+      <c r="C580" t="s">
+        <v>247</v>
+      </c>
+      <c r="D580" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="581" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A581" t="s">
+        <v>6</v>
+      </c>
+      <c r="B581">
+        <v>22800</v>
+      </c>
+      <c r="C581" t="s">
+        <v>247</v>
+      </c>
+      <c r="D581" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="582" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A582" t="s">
+        <v>6</v>
+      </c>
+      <c r="B582">
+        <v>22801</v>
+      </c>
+      <c r="C582" t="s">
+        <v>247</v>
+      </c>
+      <c r="D582" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="583" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A583" t="s">
+        <v>6</v>
+      </c>
+      <c r="B583">
+        <v>22802</v>
+      </c>
+      <c r="C583" t="s">
+        <v>247</v>
+      </c>
+      <c r="D583" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="584" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A584" t="s">
+        <v>28</v>
+      </c>
+      <c r="B584">
+        <v>21559</v>
+      </c>
+      <c r="C584" t="s">
+        <v>247</v>
+      </c>
+      <c r="D584" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="585" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A585" t="s">
+        <v>15</v>
+      </c>
+      <c r="B585">
+        <v>22803</v>
+      </c>
+      <c r="C585" t="s">
+        <v>247</v>
+      </c>
+      <c r="D585" t="s">
+        <v>485</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>